<commit_message>
Data Att + charts
</commit_message>
<xml_diff>
--- a/Q Learning Pacman/Charts - good performance.xlsx
+++ b/Q Learning Pacman/Charts - good performance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>QLearning</c:v>
+                  <c:v>Random</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -291,64 +291,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>4636</c:v>
+                  <c:v>1772.1319796954315</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4998</c:v>
+                  <c:v>1714.010152284264</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4982</c:v>
+                  <c:v>1823.6548223350253</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4350</c:v>
+                  <c:v>1727.2081218274111</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4948</c:v>
+                  <c:v>1729.2893401015228</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4526</c:v>
+                  <c:v>1782.7918781725889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4840</c:v>
+                  <c:v>1829.4923857868021</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5124</c:v>
+                  <c:v>1838.4263959390862</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5278</c:v>
+                  <c:v>1854.7715736040609</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5096</c:v>
+                  <c:v>1632.1319796954315</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4616</c:v>
+                  <c:v>1744.5685279187817</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4912</c:v>
+                  <c:v>1922.284263959391</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3802</c:v>
+                  <c:v>1804.8730964467004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4656</c:v>
+                  <c:v>1687.3604060913706</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5028</c:v>
+                  <c:v>1881.5736040609138</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4198</c:v>
+                  <c:v>1695.1776649746193</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5128</c:v>
+                  <c:v>1861.5736040609138</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4552</c:v>
+                  <c:v>1703.1472081218274</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4640</c:v>
+                  <c:v>1709.4923857868021</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5356</c:v>
+                  <c:v>1796.6497461928934</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -364,7 +364,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Random</c:v>
+                  <c:v>QLearning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -457,64 +457,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1045.2</c:v>
+                  <c:v>6269.1338582677163</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1025.2</c:v>
+                  <c:v>6464.8031496062995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>965.9</c:v>
+                  <c:v>6715.390625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1123</c:v>
+                  <c:v>6401.484375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1066.0999999999999</c:v>
+                  <c:v>6347.8125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1082</c:v>
+                  <c:v>6533.828125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1038.4000000000001</c:v>
+                  <c:v>6445.625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1016.1</c:v>
+                  <c:v>6451.171875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1127.3</c:v>
+                  <c:v>6425.15625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>986.9</c:v>
+                  <c:v>6401.953125</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1028</c:v>
+                  <c:v>6571.5625</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1124.5</c:v>
+                  <c:v>6535.234375</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1024.0999999999999</c:v>
+                  <c:v>6526.953125</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1097.5</c:v>
+                  <c:v>6424.53125</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1040</c:v>
+                  <c:v>6521.328125</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1066.0999999999999</c:v>
+                  <c:v>6506.171875</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1050.5</c:v>
+                  <c:v>6314.6875</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1091</c:v>
+                  <c:v>6212.578125</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1039.5049504950496</c:v>
+                  <c:v>6618.984375</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1028.5148514851485</c:v>
+                  <c:v>7164.84375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -529,11 +529,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="262969848"/>
-        <c:axId val="229973632"/>
+        <c:axId val="206365400"/>
+        <c:axId val="206368536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="262969848"/>
+        <c:axId val="206365400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -648,12 +648,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229973632"/>
+        <c:crossAx val="206368536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="229973632"/>
+        <c:axId val="206368536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="800"/>
@@ -767,7 +767,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262969848"/>
+        <c:crossAx val="206365400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -933,7 +933,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>QLearning</c:v>
+                  <c:v>Random</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1026,64 +1026,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.8</c:v>
+                  <c:v>6.0913705583756347E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8</c:v>
+                  <c:v>4.5685279187817257E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6</c:v>
+                  <c:v>6.0913705583756347E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6</c:v>
+                  <c:v>4.5685279187817257E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>7.1065989847715741E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6</c:v>
+                  <c:v>5.5837563451776651E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>7.1065989847715741E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8</c:v>
+                  <c:v>6.0913705583756347E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6</c:v>
+                  <c:v>7.6142131979695438E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>5.0761421319796954E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8</c:v>
+                  <c:v>6.0913705583756347E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>9.1370558375634514E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.2</c:v>
+                  <c:v>8.1218274111675121E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.8</c:v>
+                  <c:v>2.5380710659898477E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.8</c:v>
+                  <c:v>5.5837563451776651E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.8</c:v>
+                  <c:v>5.0761421319796954E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>5.0761421319796954E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6</c:v>
+                  <c:v>3.553299492385787E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2</c:v>
+                  <c:v>5.0761421319796954E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.8</c:v>
+                  <c:v>4.5685279187817257E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1099,7 +1099,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Random</c:v>
+                  <c:v>QLearning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1192,64 +1192,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.7007874015748032</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.7086614173228347</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.734375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.671875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.703125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>1.6875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>1.703125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>1.7265625</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>1.6953125</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>1.6875</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>1.703125</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>1.7578125</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>1.7265625</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>1.703125</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.99</c:v>
+                  <c:v>1.6796875</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.99</c:v>
+                  <c:v>1.6796875</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.99</c:v>
+                  <c:v>1.65625</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.99</c:v>
+                  <c:v>1.640625</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.99009900990099009</c:v>
+                  <c:v>1.7421875</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.99009900990099009</c:v>
+                  <c:v>0.9140625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1264,11 +1264,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="229972456"/>
-        <c:axId val="229972848"/>
+        <c:axId val="206366184"/>
+        <c:axId val="206367360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="229972456"/>
+        <c:axId val="206366184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -1383,12 +1383,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229972848"/>
+        <c:crossAx val="206367360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="229972848"/>
+        <c:axId val="206367360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1501,7 +1501,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229972456"/>
+        <c:crossAx val="206366184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2699,15 +2699,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2729,15 +2729,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>4763</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2762,8 +2762,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G41" totalsRowShown="0">
-  <autoFilter ref="A1:G41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G42" totalsRowShown="0">
+  <autoFilter ref="A1:G42"/>
   <sortState ref="A2:D28">
     <sortCondition ref="A1:A28"/>
   </sortState>
@@ -2773,10 +2773,10 @@
     <tableColumn id="3" name="Level"/>
     <tableColumn id="4" name="Score"/>
     <tableColumn id="5" name="Rounds"/>
-    <tableColumn id="6" name="AVG Level" dataDxfId="1">
+    <tableColumn id="6" name="AVG Level" dataDxfId="0">
       <calculatedColumnFormula>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="AVG Score" dataDxfId="0">
+    <tableColumn id="7" name="AVG Score" dataDxfId="1">
       <calculatedColumnFormula>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3050,7 +3050,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3087,32 +3087,32 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>23180</v>
+        <v>349110</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F2">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.8</v>
+        <v>6.0913705583756347E-2</v>
       </c>
       <c r="G2">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4636</v>
+        <v>1772.1319796954315</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>19</v>
@@ -3121,198 +3121,198 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>24990</v>
+        <v>337660</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F3">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.8</v>
+        <v>4.5685279187817257E-2</v>
       </c>
       <c r="G3">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4998</v>
+        <v>1714.010152284264</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>18</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>24910</v>
+        <v>359260</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F4">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.6</v>
+        <v>6.0913705583756347E-2</v>
       </c>
       <c r="G4">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4982</v>
+        <v>1823.6548223350253</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>17</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5">
-        <v>21750</v>
+        <v>340260</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F5">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.6</v>
+        <v>4.5685279187817257E-2</v>
       </c>
       <c r="G5">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4350</v>
+        <v>1727.2081218274111</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>16</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>24740</v>
+        <v>340670</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F6">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>2</v>
+        <v>7.1065989847715741E-2</v>
       </c>
       <c r="G6">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4948</v>
+        <v>1729.2893401015228</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>15</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>22630</v>
+        <v>351210</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F7">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.6</v>
+        <v>5.5837563451776651E-2</v>
       </c>
       <c r="G7">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4526</v>
+        <v>1782.7918781725889</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>14</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D8">
-        <v>24200</v>
+        <v>360410</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F8">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>2</v>
+        <v>7.1065989847715741E-2</v>
       </c>
       <c r="G8">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4840</v>
+        <v>1829.4923857868021</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>13</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D9">
-        <v>25620</v>
+        <v>362170</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F9">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.8</v>
+        <v>6.0913705583756347E-2</v>
       </c>
       <c r="G9">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>5124</v>
+        <v>1838.4263959390862</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>12</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>26390</v>
+        <v>365390</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F10">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.6</v>
+        <v>7.6142131979695438E-2</v>
       </c>
       <c r="G10">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>5278</v>
+        <v>1854.7715736040609</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>11</v>
@@ -3321,173 +3321,173 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>25480</v>
+        <v>321530</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F11">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>2</v>
+        <v>5.0761421319796954E-2</v>
       </c>
       <c r="G11">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>5096</v>
+        <v>1632.1319796954315</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D12">
-        <v>23080</v>
+        <v>343680</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F12">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.8</v>
+        <v>6.0913705583756347E-2</v>
       </c>
       <c r="G12">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4616</v>
+        <v>1744.5685279187817</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13">
         <v>9</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>24560</v>
+        <v>378690</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F13">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>2</v>
+        <v>9.1370558375634514E-2</v>
       </c>
       <c r="G13">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4912</v>
+        <v>1922.284263959391</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14">
         <v>8</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D14">
-        <v>19010</v>
+        <v>355560</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F14">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.2</v>
+        <v>8.1218274111675121E-2</v>
       </c>
       <c r="G14">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>3802</v>
+        <v>1804.8730964467004</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15">
         <v>7</v>
       </c>
       <c r="C15">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>23280</v>
+        <v>332410</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F15">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.8</v>
+        <v>2.5380710659898477E-2</v>
       </c>
       <c r="G15">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4656</v>
+        <v>1687.3604060913706</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16">
         <v>6</v>
       </c>
       <c r="C16">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D16">
-        <v>25140</v>
+        <v>370670</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F16">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.8</v>
+        <v>5.5837563451776651E-2</v>
       </c>
       <c r="G16">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>5028</v>
+        <v>1881.5736040609138</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
       <c r="C17">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17">
-        <v>20990</v>
+        <v>333950</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F17">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.8</v>
+        <v>5.0761421319796954E-2</v>
       </c>
       <c r="G17">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4198</v>
+        <v>1695.1776649746193</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -3496,48 +3496,48 @@
         <v>10</v>
       </c>
       <c r="D18">
-        <v>25640</v>
+        <v>366730</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F18">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>2</v>
+        <v>5.0761421319796954E-2</v>
       </c>
       <c r="G18">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>5128</v>
+        <v>1861.5736040609138</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
       <c r="C19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19">
-        <v>22760</v>
+        <v>335520</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F19">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1.6</v>
+        <v>3.553299492385787E-2</v>
       </c>
       <c r="G19">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4552</v>
+        <v>1703.1472081218274</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -3546,543 +3546,543 @@
         <v>10</v>
       </c>
       <c r="D20">
-        <v>23200</v>
+        <v>336770</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F20">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>2</v>
+        <v>5.0761421319796954E-2</v>
       </c>
       <c r="G20">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>4640</v>
+        <v>1709.4923857868021</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D21">
-        <v>26780</v>
+        <v>353940</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="F21">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>0.8</v>
+        <v>4.5685279187817257E-2</v>
       </c>
       <c r="G21">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>5356</v>
+        <v>1796.6497461928934</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22">
         <v>20</v>
       </c>
       <c r="C22">
-        <v>100</v>
+        <v>216</v>
       </c>
       <c r="D22">
-        <v>104520</v>
+        <v>796180</v>
       </c>
       <c r="E22">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="F22">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.7007874015748032</v>
       </c>
       <c r="G22">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1045.2</v>
+        <v>6269.1338582677163</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23">
         <v>19</v>
       </c>
       <c r="C23">
-        <v>100</v>
+        <v>217</v>
       </c>
       <c r="D23">
-        <v>102520</v>
+        <v>821030</v>
       </c>
       <c r="E23">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="F23">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.7086614173228347</v>
       </c>
       <c r="G23">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1025.2</v>
+        <v>6464.8031496062995</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24">
         <v>18</v>
       </c>
       <c r="C24">
-        <v>100</v>
+        <v>222</v>
       </c>
       <c r="D24">
-        <v>96590</v>
+        <v>859570</v>
       </c>
       <c r="E24">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F24">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.734375</v>
       </c>
       <c r="G24">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>965.9</v>
+        <v>6715.390625</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25">
         <v>17</v>
       </c>
       <c r="C25">
-        <v>100</v>
+        <v>214</v>
       </c>
       <c r="D25">
-        <v>112300</v>
+        <v>819390</v>
       </c>
       <c r="E25">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F25">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.671875</v>
       </c>
       <c r="G25">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1123</v>
+        <v>6401.484375</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26">
         <v>16</v>
       </c>
       <c r="C26">
-        <v>100</v>
+        <v>218</v>
       </c>
       <c r="D26">
-        <v>106610</v>
+        <v>812520</v>
       </c>
       <c r="E26">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F26">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.703125</v>
       </c>
       <c r="G26">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1066.0999999999999</v>
+        <v>6347.8125</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27">
         <v>15</v>
       </c>
       <c r="C27">
-        <v>100</v>
+        <v>216</v>
       </c>
       <c r="D27">
-        <v>108200</v>
+        <v>836330</v>
       </c>
       <c r="E27">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F27">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.6875</v>
       </c>
       <c r="G27">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1082</v>
+        <v>6533.828125</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28">
         <v>14</v>
       </c>
       <c r="C28">
-        <v>100</v>
+        <v>218</v>
       </c>
       <c r="D28">
-        <v>103840</v>
+        <v>825040</v>
       </c>
       <c r="E28">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F28">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.703125</v>
       </c>
       <c r="G28">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1038.4000000000001</v>
+        <v>6445.625</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29">
         <v>13</v>
       </c>
       <c r="C29">
-        <v>100</v>
+        <v>221</v>
       </c>
       <c r="D29">
-        <v>101610</v>
+        <v>825750</v>
       </c>
       <c r="E29">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F29">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.7265625</v>
       </c>
       <c r="G29">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1016.1</v>
+        <v>6451.171875</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30">
         <v>12</v>
       </c>
       <c r="C30">
-        <v>100</v>
+        <v>217</v>
       </c>
       <c r="D30">
-        <v>112730</v>
+        <v>822420</v>
       </c>
       <c r="E30">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F30">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.6953125</v>
       </c>
       <c r="G30">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1127.3</v>
+        <v>6425.15625</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B31">
         <v>11</v>
       </c>
       <c r="C31">
-        <v>100</v>
+        <v>216</v>
       </c>
       <c r="D31">
-        <v>98690</v>
+        <v>819450</v>
       </c>
       <c r="E31">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F31">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.6875</v>
       </c>
       <c r="G31">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>986.9</v>
+        <v>6401.953125</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32">
         <v>10</v>
       </c>
       <c r="C32">
-        <v>100</v>
+        <v>218</v>
       </c>
       <c r="D32">
-        <v>102800</v>
+        <v>841160</v>
       </c>
       <c r="E32">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F32">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.703125</v>
       </c>
       <c r="G32">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1028</v>
+        <v>6571.5625</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33">
         <v>9</v>
       </c>
       <c r="C33">
-        <v>100</v>
+        <v>225</v>
       </c>
       <c r="D33">
-        <v>112450</v>
+        <v>836510</v>
       </c>
       <c r="E33">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F33">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.7578125</v>
       </c>
       <c r="G33">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1124.5</v>
+        <v>6535.234375</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34">
         <v>8</v>
       </c>
       <c r="C34">
-        <v>100</v>
+        <v>221</v>
       </c>
       <c r="D34">
-        <v>102410</v>
+        <v>835450</v>
       </c>
       <c r="E34">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F34">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.7265625</v>
       </c>
       <c r="G34">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1024.0999999999999</v>
+        <v>6526.953125</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35">
         <v>7</v>
       </c>
       <c r="C35">
-        <v>100</v>
+        <v>218</v>
       </c>
       <c r="D35">
-        <v>109750</v>
+        <v>822340</v>
       </c>
       <c r="E35">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F35">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1</v>
+        <v>1.703125</v>
       </c>
       <c r="G35">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1097.5</v>
+        <v>6424.53125</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B36">
         <v>6</v>
       </c>
       <c r="C36">
-        <v>99</v>
+        <v>215</v>
       </c>
       <c r="D36">
-        <v>104000</v>
+        <v>834730</v>
       </c>
       <c r="E36">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F36">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>0.99</v>
+        <v>1.6796875</v>
       </c>
       <c r="G36">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1040</v>
+        <v>6521.328125</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37">
         <v>5</v>
       </c>
       <c r="C37">
-        <v>99</v>
+        <v>215</v>
       </c>
       <c r="D37">
-        <v>106610</v>
+        <v>832790</v>
       </c>
       <c r="E37">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F37">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>0.99</v>
+        <v>1.6796875</v>
       </c>
       <c r="G37">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1066.0999999999999</v>
+        <v>6506.171875</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B38">
         <v>4</v>
       </c>
       <c r="C38">
-        <v>99</v>
+        <v>212</v>
       </c>
       <c r="D38">
-        <v>105050</v>
+        <v>808280</v>
       </c>
       <c r="E38">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F38">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>0.99</v>
+        <v>1.65625</v>
       </c>
       <c r="G38">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1050.5</v>
+        <v>6314.6875</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
       <c r="C39">
-        <v>99</v>
+        <v>210</v>
       </c>
       <c r="D39">
-        <v>109100</v>
+        <v>795210</v>
       </c>
       <c r="E39">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F39">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>0.99</v>
+        <v>1.640625</v>
       </c>
       <c r="G39">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1091</v>
+        <v>6212.578125</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B40">
         <v>2</v>
       </c>
       <c r="C40">
-        <v>100</v>
+        <v>223</v>
       </c>
       <c r="D40">
-        <v>104990</v>
+        <v>847230</v>
       </c>
       <c r="E40">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="F40">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>0.99009900990099009</v>
+        <v>1.7421875</v>
       </c>
       <c r="G40">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1039.5049504950496</v>
+        <v>6618.984375</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="D41">
-        <v>103880</v>
+        <v>917100</v>
       </c>
       <c r="E41">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="F41">
         <f>Tabela1[[#This Row],[Level]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>0.99009900990099009</v>
+        <v>0.9140625</v>
       </c>
       <c r="G41">
         <f>Tabela1[[#This Row],[Score]]/Tabela1[[#This Row],[Rounds]]</f>
-        <v>1028.5148514851485</v>
+        <v>7164.84375</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>